<commit_message>
Update LL table to include empty lines
</commit_message>
<xml_diff>
--- a/docs/LL_Table.xlsx
+++ b/docs/LL_Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\fakt_skola\3 BIT\IFJ\projekt\IFJ18\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SharedProjects\IFJ18\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204678FE-1C36-4D72-9D84-A8D37193FA0B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA8D389-B792-470A-9EE5-B69A16BA8AC3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5640" xr2:uid="{04AF779E-42B5-4928-B194-5F22BF2ACE98}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="117">
   <si>
     <t>&lt;prog&gt;</t>
   </si>
@@ -246,9 +246,6 @@
     <t>eol</t>
   </si>
   <si>
-    <t>{id, while if, def}</t>
-  </si>
-  <si>
     <t>{id, (}</t>
   </si>
   <si>
@@ -366,9 +363,6 @@
     <t>33. &lt;value&gt; → STRING</t>
   </si>
   <si>
-    <t>{id, while, if, $}</t>
-  </si>
-  <si>
     <t>{string, id, float, int, (, eol}</t>
   </si>
   <si>
@@ -379,19 +373,35 @@
   </si>
   <si>
     <t>9. &lt;statement&gt; → while &lt;expression&gt; do EOL &lt;statement&gt; end EOL  &lt;statement&gt;</t>
+  </si>
+  <si>
+    <t>34.  &lt;statenemt&gt; → EOL &lt;statement&gt;</t>
+  </si>
+  <si>
+    <t>{id, while if, def, eol}</t>
+  </si>
+  <si>
+    <t>{id, while, if, $, eol}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -560,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -569,38 +579,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -917,23 +933,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D8F368-A862-40F3-80B0-4AA651053DE9}">
-  <dimension ref="A1:AH42"/>
+  <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="89.5703125" customWidth="1"/>
-    <col min="7" max="7" width="67.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.15625" customWidth="1"/>
+    <col min="3" max="3" width="65.68359375" customWidth="1"/>
+    <col min="4" max="4" width="17.68359375" customWidth="1"/>
+    <col min="6" max="6" width="89.578125" customWidth="1"/>
+    <col min="7" max="7" width="67.15625" customWidth="1"/>
+    <col min="9" max="9" width="15.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
@@ -1023,7 +1039,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1047,7 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -1051,7 +1067,9 @@
       <c r="K2" s="6">
         <v>2</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="21">
+        <v>2</v>
+      </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -1081,7 +1099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1089,16 +1107,16 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>1</v>
@@ -1137,7 +1155,7 @@
       <c r="AG3" s="7"/>
       <c r="AH3" s="7"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1145,7 +1163,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>66</v>
@@ -1185,7 +1203,7 @@
       <c r="AG4" s="8"/>
       <c r="AH4" s="8"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1214,7 @@
         <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
         <v>55</v>
@@ -1211,7 +1229,9 @@
       <c r="K5" s="9">
         <v>10</v>
       </c>
-      <c r="L5" s="9"/>
+      <c r="L5" s="20">
+        <v>34</v>
+      </c>
       <c r="M5" s="9">
         <v>11</v>
       </c>
@@ -1245,7 +1265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -1253,16 +1273,16 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
         <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>4</v>
@@ -1313,7 +1333,7 @@
       <c r="AG6" s="10"/>
       <c r="AH6" s="10"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
@@ -1321,16 +1341,16 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
         <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>5</v>
@@ -1375,7 +1395,7 @@
       </c>
       <c r="AH7" s="11"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1383,10 +1403,10 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>7</v>
@@ -1423,7 +1443,7 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="12"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1431,10 +1451,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
         <v>58</v>
@@ -1479,7 +1499,7 @@
       </c>
       <c r="AH9" s="13"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1487,16 +1507,16 @@
         <v>29</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>68</v>
@@ -1541,7 +1561,7 @@
       </c>
       <c r="AH10" s="19"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1552,10 +1572,10 @@
         <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1566,13 +1586,13 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1580,16 +1600,16 @@
         <v>29</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>70</v>
       </c>
@@ -1597,16 +1617,16 @@
         <v>29</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1617,13 +1637,13 @@
         <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1634,7 +1654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1645,13 +1665,13 @@
         <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1662,13 +1682,13 @@
         <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -1679,7 +1699,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1690,13 +1710,13 @@
         <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -1707,13 +1727,13 @@
         <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -1724,13 +1744,13 @@
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -1741,13 +1761,13 @@
         <v>41</v>
       </c>
       <c r="F23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1758,13 +1778,13 @@
         <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -1775,13 +1795,13 @@
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1792,13 +1812,13 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1809,13 +1829,13 @@
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -1826,13 +1846,13 @@
         <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1843,13 +1863,13 @@
         <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1860,13 +1880,13 @@
         <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1877,7 +1897,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1888,13 +1908,13 @@
         <v>49</v>
       </c>
       <c r="F32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
@@ -1902,16 +1922,16 @@
         <v>29</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G33" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -1919,16 +1939,16 @@
         <v>29</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="16" t="s">
         <v>64</v>
       </c>
@@ -1936,60 +1956,69 @@
         <v>29</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="18"/>
       <c r="F36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G36" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="17"/>
       <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F39" t="s">
         <v>106</v>
       </c>
-      <c r="G37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F39" t="s">
+      <c r="G39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F40" t="s">
         <v>107</v>
       </c>
-      <c r="G39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F40" t="s">
+      <c r="G40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41" t="s">
         <v>108</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F41" t="s">
-        <v>109</v>
-      </c>
-      <c r="G41" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F44" t="s">
+        <v>114</v>
+      </c>
+      <c r="G44" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F42" t="s">
-        <v>110</v>
-      </c>
-      <c r="G42" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add rule for EOL
</commit_message>
<xml_diff>
--- a/docs/LL_Table.xlsx
+++ b/docs/LL_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SharedProjects\IFJ18\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA8D389-B792-470A-9EE5-B69A16BA8AC3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0267D83C-24C7-42E8-9663-04DF0E94D0D1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5640" xr2:uid="{04AF779E-42B5-4928-B194-5F22BF2ACE98}"/>
   </bookViews>
@@ -936,7 +936,7 @@
   <dimension ref="A1:AH44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Correct and implement grammar
</commit_message>
<xml_diff>
--- a/docs/LL_Table.xlsx
+++ b/docs/LL_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\fakt_skola\3 BIT\IFJ\projekt\IFJ18\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B23943-4ABC-4B84-935D-6642A95AC536}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85F0C6A-C626-4983-8568-15672B52A6EF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5640" xr2:uid="{04AF779E-42B5-4928-B194-5F22BF2ACE98}"/>
   </bookViews>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D8F368-A862-40F3-80B0-4AA651053DE9}">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>